<commit_message>
2023-07-04 Tuesday, 15:35:22 Auto Push
</commit_message>
<xml_diff>
--- a/2023-07-04 Tuesday.xlsx
+++ b/2023-07-04 Tuesday.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,30 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>303</v>
+      </c>
+      <c r="B2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>王*佑</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2023-07-04 15:27:23</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
2023-07-04 Tuesday, 16:35:25 Auto Push
</commit_message>
<xml_diff>
--- a/2023-07-04 Tuesday.xlsx
+++ b/2023-07-04 Tuesday.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,13 +479,41 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2023-07-04 15:27:23</t>
+          <t>2023-07-04 16:32:08</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
           <t>IN</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>303</v>
+      </c>
+      <c r="B3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>王*佑</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2023-07-04 15:27:23</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2023-07-04 15:42:50</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>OUT</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
2023-07-04 Tuesday, 17:35:29 Auto Push
</commit_message>
<xml_diff>
--- a/2023-07-04 Tuesday.xlsx
+++ b/2023-07-04 Tuesday.xlsx
@@ -482,10 +482,14 @@
           <t>2023-07-04 16:32:08</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2023-07-04 17:04:03</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>OUT</t>
         </is>
       </c>
     </row>

</xml_diff>